<commit_message>
Changed anagnostopoulos to fidaner. - Capitalized first letter of all daltonization methods. - Cahnged default MaxIter in imgRecolor.m to 500. - Cleaned up callImgRecolorFromPython.m. - Cahnged scene to motive, and version to variant in visualsearch_ids.csv and visualsearch_ids.xlsx.
</commit_message>
<xml_diff>
--- a/colordeficiency-data/visualsearch_ids.xlsx
+++ b/colordeficiency-data/visualsearch_ids.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21720" windowHeight="18800" tabRatio="500"/>
@@ -24,13 +24,13 @@
     <t>image_id</t>
   </si>
   <si>
-    <t>scene_id</t>
+    <t>set_id</t>
   </si>
   <si>
-    <t>version_id</t>
+    <t>motive_id</t>
   </si>
   <si>
-    <t>set_id</t>
+    <t>variant_id</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -448,13 +448,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>